<commit_message>
Ajout du scoutisme marin #26
</commit_message>
<xml_diff>
--- a/fichiers/conf/modele_marins.xlsx
+++ b/fichiers/conf/modele_marins.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\analytiscout\fichiers\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6AE97CE-7C60-4218-9AAC-AD9AED8CB259}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8D10CE6-3064-40C7-9567-7B36ABA66DE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3285" yWindow="285" windowWidth="24495" windowHeight="13410" tabRatio="391" activeTab="1" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
+    <workbookView xWindow="1230" yWindow="495" windowWidth="25125" windowHeight="13410" tabRatio="391" activeTab="1" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Aide" sheetId="4" r:id="rId1"/>
@@ -149,15 +149,6 @@
     <t>Diplômes</t>
   </si>
   <si>
-    <t>PE</t>
-  </si>
-  <si>
-    <t>CQ</t>
-  </si>
-  <si>
-    <t>CF</t>
-  </si>
-  <si>
     <t>${chef.formation.pe.datefin}</t>
   </si>
   <si>
@@ -201,6 +192,15 @@
   </si>
   <si>
     <t>Aide pour l'analyse des marins</t>
+  </si>
+  <si>
+    <t>Patron d'embarcation</t>
+  </si>
+  <si>
+    <t>Chef de quart</t>
+  </si>
+  <si>
+    <t>Chef de flottille</t>
   </si>
 </sst>
 </file>
@@ -1039,13 +1039,13 @@
   <sheetData>
     <row r="1" spans="1:1" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:1" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:1" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:1" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1095,7 +1095,13 @@
     <col min="6" max="6" width="12.28515625" style="1" customWidth="1"/>
     <col min="7" max="7" width="10" style="1" customWidth="1"/>
     <col min="8" max="8" width="3.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="16" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="12.85546875" style="1" customWidth="1"/>
     <col min="12" max="12" width="2.7109375" customWidth="1"/>
+    <col min="13" max="13" width="16.42578125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="12.140625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="12.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1117,7 +1123,7 @@
       <c r="N1" s="27"/>
       <c r="O1" s="28"/>
     </row>
-    <row r="2" spans="1:15" s="16" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" s="16" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
@@ -1137,31 +1143,31 @@
         <v>19</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="H2" s="12" t="s">
         <v>22</v>
       </c>
       <c r="I2" s="18" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="J2" s="18" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="K2" s="18" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="L2" s="12" t="s">
         <v>22</v>
       </c>
       <c r="M2" s="19" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="N2" s="19" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="O2" s="19" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -1187,22 +1193,22 @@
         <v>33</v>
       </c>
       <c r="I3" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="K3" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="M3" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="J3" s="17" t="s">
+      <c r="N3" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="K3" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="M3" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="N3" s="17" t="s">
-        <v>43</v>
-      </c>
       <c r="O3" s="17" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1303,10 +1309,12 @@
     <col min="6" max="6" width="12.28515625" style="1" customWidth="1"/>
     <col min="7" max="7" width="8.140625" style="1" customWidth="1"/>
     <col min="8" max="8" width="3.5703125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="16.85546875" customWidth="1"/>
     <col min="12" max="12" width="2.7109375" customWidth="1"/>
+    <col min="13" max="13" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="29"/>
       <c r="B1" s="30"/>
       <c r="C1" s="30"/>
@@ -1325,7 +1333,7 @@
       <c r="N1" s="27"/>
       <c r="O1" s="28"/>
     </row>
-    <row r="2" spans="1:15" s="16" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" s="16" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
@@ -1351,25 +1359,25 @@
         <v>22</v>
       </c>
       <c r="I2" s="18" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="J2" s="18" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="K2" s="18" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="L2" s="12" t="s">
         <v>22</v>
       </c>
       <c r="M2" s="19" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="N2" s="19" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="O2" s="19" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -1396,22 +1404,22 @@
       </c>
       <c r="H3" s="9"/>
       <c r="I3" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="J3" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="K3" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="M3" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="J3" s="17" t="s">
+      <c r="N3" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="K3" s="17" t="s">
+      <c r="O3" s="17" t="s">
         <v>46</v>
-      </c>
-      <c r="M3" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="N3" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="O3" s="17" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>